<commit_message>
main functionalities are converted into functions, and got triggered from main.py, need to covert main.py to hold fastapi code
</commit_message>
<xml_diff>
--- a/dc2.xlsx
+++ b/dc2.xlsx
@@ -3961,9 +3961,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>192240</xdr:colOff>
+      <xdr:colOff>191880</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>131040</xdr:rowOff>
+      <xdr:rowOff>130680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3972,8 +3972,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2534760" y="5087520"/>
-          <a:ext cx="80640" cy="110880"/>
+          <a:off x="2862360" y="5087520"/>
+          <a:ext cx="80280" cy="110520"/>
         </a:xfrm>
         <a:prstGeom prst="star5">
           <a:avLst>
@@ -4018,9 +4018,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>206280</xdr:colOff>
+      <xdr:colOff>205920</xdr:colOff>
       <xdr:row>1191</xdr:row>
-      <xdr:rowOff>146160</xdr:rowOff>
+      <xdr:rowOff>145800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4029,8 +4029,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2534760" y="215582040"/>
-          <a:ext cx="94680" cy="105480"/>
+          <a:off x="2862360" y="215582040"/>
+          <a:ext cx="94320" cy="105120"/>
         </a:xfrm>
         <a:prstGeom prst="star5">
           <a:avLst>
@@ -9564,7 +9564,7 @@
         <v>211.52</v>
       </c>
       <c r="F231" s="5" t="n">
-        <v>265</v>
+        <v>230</v>
       </c>
       <c r="G231" s="6" t="n">
         <v>125</v>

</xml_diff>